<commit_message>
Tracklet version 2 (Train)
</commit_message>
<xml_diff>
--- a/tracklets/train/022.xlsx
+++ b/tracklets/train/022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/as16542/OneDrive - University of Bristol/Repositories/Metric Learning Open Cows/tracklets/train/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B2953E-1DBB-E345-B582-03BB8E264917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D772954E-3CC4-FE40-9A1E-B84CD7D48CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1345,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1359,30 +1359,48 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" spans="1:2" ht="92" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:2" ht="92" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="92" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:2" ht="92" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:2" ht="92" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="92" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>